<commit_message>
PROS-6604 - MARSRU kpis 2019
</commit_message>
<xml_diff>
--- a/Projects/MARSRU_PROD/Data/2019/KPIs for DB - MARS KPIs.xlsx
+++ b/Projects/MARSRU_PROD/Data/2019/KPIs for DB - MARS KPIs.xlsx
@@ -301,17 +301,17 @@
   </sheetPr>
   <dimension ref="A1:D65"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D50" activeCellId="0" sqref="D50"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C51" activeCellId="0" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.1734693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.2397959183673"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.1275510204082"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="222.872448979592"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.6326530612245"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.8316326530612"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.7244897959184"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="220.438775510204"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1000,29 +1000,29 @@
         <v>52</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
         <v>4</v>
       </c>
       <c r="B50" s="2" t="n">
-        <v>4310</v>
+        <v>4697</v>
       </c>
       <c r="C50" s="2" t="n">
-        <v>4310</v>
+        <v>4697</v>
       </c>
       <c r="D50" s="0" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
         <v>4</v>
       </c>
       <c r="B51" s="2" t="n">
-        <v>4330</v>
+        <v>4698</v>
       </c>
       <c r="C51" s="2" t="n">
-        <v>4330</v>
+        <v>4698</v>
       </c>
       <c r="D51" s="0" t="s">
         <v>54</v>

</xml_diff>

<commit_message>
PROS-6604 - MARSRU kpis 2019 - SD-65824
</commit_message>
<xml_diff>
--- a/Projects/MARSRU_PROD/Data/2019/KPIs for DB - MARS KPIs.xlsx
+++ b/Projects/MARSRU_PROD/Data/2019/KPIs for DB - MARS KPIs.xlsx
@@ -136,16 +136,16 @@
     <t xml:space="preserve">Выкладка Марс вертикальными бренд-блоками, которые стремятся к прямоугольнику, с четким разделением на типы продукта (сухой/влажный)</t>
   </si>
   <si>
-    <t xml:space="preserve">Категория выстроена либо в единую линию, либо в две линии строго друг напротив друга (лицом друг к другу)</t>
+    <t xml:space="preserve">Есть ЦА: Категория выстроена либо в единую линию, либо в две линии строго друг напротив друга (лицом друг к другу)</t>
   </si>
   <si>
     <t xml:space="preserve">В магазине есть центральная аллея (ЦА)</t>
   </si>
   <si>
-    <t xml:space="preserve">Категория тов. для животных примыкает к ЦЕНТРАЛЬНОЙ АЛЛЕЕ и визуально доступна покупателям по ходу их движения без необходимости оборачиваться</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Категория товаров для животных примыкает к ПРОМО АЛЛЕЕ, находится дальше 5-ти метров от входа и визуально доступна покупателям по ходу их движения без необходимости оборачиваться</t>
+    <t xml:space="preserve">Есть ЦА: Категория товаров для животных примыкает к ЦЕНТРАЛЬНОЙ АЛЛЕЕ и визуально доступна покупателям по ходу их движения без необходимости оборачиваться</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Есть ЦА: Категория товаров для животных примыкает к ПРОМО АЛЛЕЕ, находится дальше 5-ти метров от входа и визуально доступна покупателям по ходу их движения без необходимости оборачиваться</t>
   </si>
   <si>
     <t xml:space="preserve">Ассортимент для Котят/Щенков, а также Senior сгруппирован (влажный и сухой) и располагается внутри соответствующих бренд блоков </t>
@@ -301,17 +301,16 @@
   </sheetPr>
   <dimension ref="A1:D65"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C51" activeCellId="0" sqref="C51"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D38" activeCellId="0" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.6326530612245"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.8316326530612"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.7244897959184"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="220.438775510204"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.0918367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.4285714285714"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.3163265306122"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="218.010204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
PROS-7602 - MARSRU - Drogerie channel KPIs
</commit_message>
<xml_diff>
--- a/Projects/MARSRU_PROD/Data/2019/KPIs for DB - MARS KPIs.xlsx
+++ b/Projects/MARSRU_PROD/Data/2019/KPIs for DB - MARS KPIs.xlsx
@@ -8,7 +8,8 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="76">
   <si>
     <t xml:space="preserve">KPI Level 1 Name</t>
   </si>
@@ -37,6 +38,78 @@
     <t xml:space="preserve">MARS KPIs</t>
   </si>
   <si>
+    <t xml:space="preserve">Категория кормов размещается в первом зале по ходу движения покупателя (Drogerie SS) или в радиусе 3-х метров от места расчета (Drogerie BTC)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Категория кормов примыкает или находится в радиусе 3-х метров от центра выкладки одной из приоритетных категорий так, что видны блоки паучей Kitekat и Whiskas  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Категория располагается вне тупика и находится дальше 3м от входа/выхода</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Суммарный размер выкладки МАРС (в метрах) на всех полках для категорий кошки (включая лакомства на основной полке, БЕЗ Catsan)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Суммарный размер выкладки всей категории (в метрах)на всех полках для категорий кошки (включая лакомства на основной полке, БЕЗ НАПОЛНИТЕЛЕЙ)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Суммарный размер выкладки МАРС (в метрах) на всех полках для категорий собаки (включая лакомства на основной полке)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Суммарный размер выкладки всей категории (в метрах) на всех полках для категорий собаки (включая лакомства на основной полке)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">В торговой точке присутствует хотя бы 1 линия кормов Марс</t>
+  </si>
+  <si>
+    <t xml:space="preserve">В торговой точке присутствует базовый Must Range (35 SKU)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">В торговой точке присутствует кластерный Must Range (5 SKU)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">В торговой точке есть ДМП Марс (с продукцией cat пауч + лакомства) в прикассовой зоне или в приоритетной категории</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Наличие лакомств SKU 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Наличие лакомств SKU 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Наличие лакомств SKU 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Наличие лакомств SKU 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Наличие лакомств SKU 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Наличие лакомств SKU 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Наличие лакомств SKU 7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Выкладка Марс вертикальными бренд-блоками, которые стремятся к прямоугольным, с четким разделением на типы продукта (сухой/влажный)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Влажные корма Марс внутри выкладки кошек располагаются в следующем порядке: Китекат-Вискас-Шеба мини-пауч-Перфект Фит  -Шеба пауч, Nature’s Table, Шеба трэй (допускается выкладка Шеба единым блоком на малых полках)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Whiskas и Kitekat pouch располагаются рядом - единым неразрывным блоком</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Большая дюжина - 12 SKU расположены в соответствии с планограммой (не ниже 3-й полки и не выше 7-й)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ассортимент для Котят/Щенков, а также Senior сгруппирован (влажный и сухой) и располагается внутри соответствующих бренд блоков</t>
+  </si>
+  <si>
+    <t xml:space="preserve">В магазине тип выкладки А</t>
+  </si>
+  <si>
     <t xml:space="preserve">Среднее кол-во полок c кормами и лакомствами для кошек на стеллаже</t>
   </si>
   <si>
@@ -97,21 +170,9 @@
     <t xml:space="preserve">Суммарный линейный размер влажных однопорционных кормов  Perfect Fit + Sheba  минимум на 40% больше любого другого суперпремиального бренда</t>
   </si>
   <si>
-    <t xml:space="preserve">Большая дюжина - 12 SKU расположены в соответствии с планограммой (не ниже 3-й полки и не выше 7-й)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Суммарный размер выкладки МАРС (в метрах) на всех полках для категорий кошки (включая лакомства на основной полке, БЕЗ Catsan)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Суммарный размер выкладки всей категории (в метрах)на всех полках для категорий кошки (включая лакомства на основной полке, БЕЗ НАПОЛНИТЕЛЕЙ)</t>
-  </si>
-  <si>
     <t xml:space="preserve">В торговой точке присутствует частная марка в категории кошки</t>
   </si>
   <si>
-    <t xml:space="preserve">Суммарный размер выкладки МАРС (в метрах) на всех полках для категорий собаки (включая лакомства на основной полке)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Суммарный размер выкладки всей категории (в метрах)на всех полках для категорий собаки (включая лакомства на основной полке)</t>
   </si>
   <si>
@@ -136,24 +197,21 @@
     <t xml:space="preserve">Выкладка Марс вертикальными бренд-блоками, которые стремятся к прямоугольнику, с четким разделением на типы продукта (сухой/влажный)</t>
   </si>
   <si>
-    <t xml:space="preserve">Есть ЦА: Категория выстроена либо в единую линию, либо в две линии строго друг напротив друга (лицом друг к другу)</t>
+    <t xml:space="preserve">Категория выстроена либо в единую линию, либо в две линии строго друг напротив друга (лицом друг к другу)</t>
   </si>
   <si>
     <t xml:space="preserve">В магазине есть центральная аллея (ЦА)</t>
   </si>
   <si>
-    <t xml:space="preserve">Есть ЦА: Категория товаров для животных примыкает к ЦЕНТРАЛЬНОЙ АЛЛЕЕ и визуально доступна покупателям по ходу их движения без необходимости оборачиваться</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Есть ЦА: Категория товаров для животных примыкает к ПРОМО АЛЛЕЕ, находится дальше 5-ти метров от входа и визуально доступна покупателям по ходу их движения без необходимости оборачиваться</t>
+    <t xml:space="preserve">Категория тов. для животных примыкает к ЦЕНТРАЛЬНОЙ АЛЛЕЕ и визуально доступна покупателям по ходу их движения без необходимости оборачиваться</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Категория товаров для животных примыкает к ПРОМО АЛЛЕЕ, находится дальше 5-ти метров от входа и визуально доступна покупателям по ходу их движения без необходимости оборачиваться </t>
   </si>
   <si>
     <t xml:space="preserve">Ассортимент для Котят/Щенков, а также Senior сгруппирован (влажный и сухой) и располагается внутри соответствующих бренд блоков </t>
   </si>
   <si>
-    <t xml:space="preserve">Влажные корма Марс внутри выкладки кошек располагаются в следующем порядке: Китекат-Вискас-Шеба мини-пауч-Перфект Фит  -Шеба пауч, Nature’s Table, Шеба трэй (допускается выкладка Шеба единым блоком на малых полках)</t>
-  </si>
-  <si>
     <t xml:space="preserve">В наличии ценники для каждого SKU</t>
   </si>
   <si>
@@ -191,18 +249,6 @@
   </si>
   <si>
     <t xml:space="preserve">В торговой точке В ПРИЛЕГАЮЩЕЙ К КАССАМ ЗОНЕ присутствуют лакомства для кошек и/или собак компании Марс</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Нет ЦА: Категория тов. для животных примыкает или расположена в радиусе 5 м от центра выкладки приоритетной категории (1) (молочные прод, фрукты и овощи, хлебобулочные изд, кондитерские изд, мясн. изд. и рыба) таким образом, что видны блоки паучей Kitekat и Whiskas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Нет ЦА: Категория товаров для животных примыкает или расположена в радиусе 5 м от центра выкладки приоритетной категории (2) (консервы, соки, вода/газированные напитки, замороженные продукты), таким образом, что видны блоки паучей Kitekat  и Whiskas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Нет ЦА: Категория выстроена в единую линию единым блоком или образует внутренний угол</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Нет ЦА: Категория располагается вне тупика и находится дальше 5 м от входа/выхода и кассовой зоны</t>
   </si>
 </sst>
 </file>
@@ -311,18 +357,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D65"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A55" activeCellId="0" sqref="A55"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D27" activeCellId="0" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.6887755102041"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.0255102040816"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.9132653061224"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="215.581632653061"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.7142857142857"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.6428571428571"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.530612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="225.301020408163"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
@@ -340,7 +386,388 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>4259</v>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>4259</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>4200</v>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>4200</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>4260</v>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>4260</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="n">
+        <v>4269</v>
+      </c>
+      <c r="C5" s="2" t="n">
+        <v>4269</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>4270</v>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>4270</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="2" t="n">
+        <v>4271</v>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>4271</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="2" t="n">
+        <v>4272</v>
+      </c>
+      <c r="C8" s="2" t="n">
+        <v>4272</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="2" t="n">
+        <v>4358</v>
+      </c>
+      <c r="C9" s="2" t="n">
+        <v>4358</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="2" t="n">
+        <v>4388</v>
+      </c>
+      <c r="C10" s="2" t="n">
+        <v>4388</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="2" t="n">
+        <v>4389</v>
+      </c>
+      <c r="C11" s="2" t="n">
+        <v>4389</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="2" t="n">
+        <v>4636</v>
+      </c>
+      <c r="C12" s="2" t="n">
+        <v>4636</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="2" t="n">
+        <v>4669</v>
+      </c>
+      <c r="C13" s="2" t="n">
+        <v>4669</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="2" t="n">
+        <v>4670</v>
+      </c>
+      <c r="C14" s="2" t="n">
+        <v>4670</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="2" t="n">
+        <v>4671</v>
+      </c>
+      <c r="C15" s="2" t="n">
+        <v>4671</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="2" t="n">
+        <v>4672</v>
+      </c>
+      <c r="C16" s="2" t="n">
+        <v>4672</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="2" t="n">
+        <v>4673</v>
+      </c>
+      <c r="C17" s="2" t="n">
+        <v>4673</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="2" t="n">
+        <v>4674</v>
+      </c>
+      <c r="C18" s="2" t="n">
+        <v>4674</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="2" t="n">
+        <v>4675</v>
+      </c>
+      <c r="C19" s="2" t="n">
+        <v>4675</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" s="2" t="n">
+        <v>4647</v>
+      </c>
+      <c r="C20" s="2" t="n">
+        <v>4647</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" s="2" t="n">
+        <v>4648</v>
+      </c>
+      <c r="C21" s="2" t="n">
+        <v>4648</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" s="2" t="n">
+        <v>4649</v>
+      </c>
+      <c r="C22" s="2" t="n">
+        <v>4649</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" s="2" t="n">
+        <v>4650</v>
+      </c>
+      <c r="C23" s="2" t="n">
+        <v>4650</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24" s="2" t="n">
+        <v>4651</v>
+      </c>
+      <c r="C24" s="2" t="n">
+        <v>4651</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" s="2" t="n">
+        <v>4704</v>
+      </c>
+      <c r="C25" s="2" t="n">
+        <v>4704</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D53"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A39" activeCellId="0" sqref="A39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.7142857142857"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.6428571428571"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.530612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="225.301020408163"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>4</v>
       </c>
@@ -351,10 +778,10 @@
         <v>4264</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>4</v>
       </c>
@@ -365,10 +792,10 @@
         <v>4351</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>4</v>
       </c>
@@ -379,10 +806,10 @@
         <v>4783</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>4</v>
       </c>
@@ -393,10 +820,10 @@
         <v>4784</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>4</v>
       </c>
@@ -407,10 +834,10 @@
         <v>4785</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>4</v>
       </c>
@@ -421,10 +848,10 @@
         <v>4268</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>4</v>
       </c>
@@ -435,10 +862,10 @@
         <v>4273</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>4</v>
       </c>
@@ -449,10 +876,10 @@
         <v>4274</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>4</v>
       </c>
@@ -463,10 +890,10 @@
         <v>4276</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>4</v>
       </c>
@@ -477,10 +904,10 @@
         <v>4282</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>4</v>
       </c>
@@ -491,10 +918,10 @@
         <v>4284</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
         <v>4</v>
       </c>
@@ -505,10 +932,10 @@
         <v>4285</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
         <v>4</v>
       </c>
@@ -519,10 +946,10 @@
         <v>4275</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
         <v>4</v>
       </c>
@@ -533,10 +960,10 @@
         <v>4277</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
         <v>4</v>
       </c>
@@ -547,10 +974,10 @@
         <v>4283</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
         <v>4</v>
       </c>
@@ -561,10 +988,10 @@
         <v>4510</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
         <v>4</v>
       </c>
@@ -575,10 +1002,10 @@
         <v>4511</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
         <v>4</v>
       </c>
@@ -589,10 +1016,10 @@
         <v>4254</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
         <v>4</v>
       </c>
@@ -603,10 +1030,10 @@
         <v>4513</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
         <v>4</v>
       </c>
@@ -617,10 +1044,10 @@
         <v>4514</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
         <v>4</v>
       </c>
@@ -631,10 +1058,10 @@
         <v>4317</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
         <v>4</v>
       </c>
@@ -645,10 +1072,10 @@
         <v>4261</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
         <v>4</v>
       </c>
@@ -659,10 +1086,10 @@
         <v>4262</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
         <v>4</v>
       </c>
@@ -673,10 +1100,10 @@
         <v>4263</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
         <v>4</v>
       </c>
@@ -687,10 +1114,10 @@
         <v>4265</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
         <v>4</v>
       </c>
@@ -701,10 +1128,10 @@
         <v>4266</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
         <v>4</v>
       </c>
@@ -715,10 +1142,10 @@
         <v>4255</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
         <v>4</v>
       </c>
@@ -729,10 +1156,10 @@
         <v>4148</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
         <v>4</v>
       </c>
@@ -743,10 +1170,10 @@
         <v>4149</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
         <v>4</v>
       </c>
@@ -757,10 +1184,10 @@
         <v>4150</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
         <v>4</v>
       </c>
@@ -771,10 +1198,10 @@
         <v>4267</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
         <v>4</v>
       </c>
@@ -785,10 +1212,10 @@
         <v>4305</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
         <v>4</v>
       </c>
@@ -799,10 +1226,10 @@
         <v>4306</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
         <v>4</v>
       </c>
@@ -813,10 +1240,10 @@
         <v>4191</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
         <v>4</v>
       </c>
@@ -827,10 +1254,10 @@
         <v>4688</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
         <v>4</v>
       </c>
@@ -841,7 +1268,7 @@
         <v>4256</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -855,7 +1282,7 @@
         <v>4219</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -869,7 +1296,7 @@
         <v>4307</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>42</v>
+        <v>62</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -883,10 +1310,10 @@
         <v>4315</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
         <v>4</v>
       </c>
@@ -897,10 +1324,10 @@
         <v>4318</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
         <v>4</v>
       </c>
@@ -911,10 +1338,10 @@
         <v>4512</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
         <v>4</v>
       </c>
@@ -925,10 +1352,10 @@
         <v>4515</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
         <v>4</v>
       </c>
@@ -939,10 +1366,10 @@
         <v>4316</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
         <v>4</v>
       </c>
@@ -953,10 +1380,10 @@
         <v>90001</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
         <v>4</v>
       </c>
@@ -967,10 +1394,10 @@
         <v>90002</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
         <v>4</v>
       </c>
@@ -981,10 +1408,10 @@
         <v>90003</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
         <v>4</v>
       </c>
@@ -995,10 +1422,10 @@
         <v>2537</v>
       </c>
       <c r="D48" s="0" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
         <v>4</v>
       </c>
@@ -1009,7 +1436,7 @@
         <v>2527</v>
       </c>
       <c r="D49" s="0" t="s">
-        <v>52</v>
+        <v>71</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1017,13 +1444,13 @@
         <v>4</v>
       </c>
       <c r="B50" s="2" t="n">
-        <v>4697</v>
+        <v>4310</v>
       </c>
       <c r="C50" s="2" t="n">
-        <v>4697</v>
+        <v>4310</v>
       </c>
       <c r="D50" s="0" t="s">
-        <v>53</v>
+        <v>72</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1031,16 +1458,16 @@
         <v>4</v>
       </c>
       <c r="B51" s="2" t="n">
-        <v>4698</v>
+        <v>4330</v>
       </c>
       <c r="C51" s="2" t="n">
-        <v>4698</v>
+        <v>4330</v>
       </c>
       <c r="D51" s="0" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
         <v>4</v>
       </c>
@@ -1051,7 +1478,7 @@
         <v>4630</v>
       </c>
       <c r="D52" s="0" t="s">
-        <v>55</v>
+        <v>74</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1065,79 +1492,9 @@
         <v>4631</v>
       </c>
       <c r="D53" s="0" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="B54" s="2" t="n">
-        <v>4601</v>
-      </c>
-      <c r="C54" s="2" t="n">
-        <v>4601</v>
-      </c>
-      <c r="D54" s="0" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="B55" s="2" t="n">
-        <v>4602</v>
-      </c>
-      <c r="C55" s="2" t="n">
-        <v>4602</v>
-      </c>
-      <c r="D55" s="0" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="B56" s="2" t="n">
-        <v>4603</v>
-      </c>
-      <c r="C56" s="2" t="n">
-        <v>4603</v>
-      </c>
-      <c r="D56" s="0" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="B57" s="2" t="n">
-        <v>4604</v>
-      </c>
-      <c r="C57" s="2" t="n">
-        <v>4604</v>
-      </c>
-      <c r="D57" s="0" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="62" customFormat="false" ht="55.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="63" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="64" customFormat="false" ht="41.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="65" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="66" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="67" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="68" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="69" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="70" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="71" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>75</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>